<commit_message>
backup on Dec 13 , 2021
</commit_message>
<xml_diff>
--- a/phase_04/v1.6_for_thesis_report/res_compiled.xlsx
+++ b/phase_04/v1.6_for_thesis_report/res_compiled.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12510" tabRatio="201" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="27795" windowHeight="12510" tabRatio="201" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3108,8 +3108,8 @@
   <sheetPr/>
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75"/>
@@ -3560,8 +3560,8 @@
   <sheetPr/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75"/>
@@ -3658,16 +3658,16 @@
         <v>69.07</v>
       </c>
       <c r="F4" s="11">
-        <v>73.52</v>
+        <v>76.37</v>
       </c>
       <c r="G4" s="11">
-        <v>2.07</v>
+        <v>1.825</v>
       </c>
       <c r="H4" s="11">
-        <v>70.23</v>
+        <v>71.4</v>
       </c>
       <c r="I4" s="14">
-        <v>78.57</v>
+        <v>79.36</v>
       </c>
     </row>
     <row r="6" spans="1:1">

</xml_diff>

<commit_message>
backup on 21 dec 2021
</commit_message>
<xml_diff>
--- a/phase_04/v1.6_for_thesis_report/res_compiled.xlsx
+++ b/phase_04/v1.6_for_thesis_report/res_compiled.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12510" tabRatio="201" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12510" tabRatio="334" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AF$2</definedName>
@@ -675,11 +676,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -736,8 +737,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -751,26 +768,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -783,30 +792,16 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,9 +815,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -835,14 +836,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -850,11 +843,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -897,7 +898,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -909,7 +910,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,19 +940,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -945,73 +1036,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1023,43 +1054,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1166,11 +1167,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1190,6 +1197,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1201,17 +1217,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1231,21 +1236,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1254,147 +1244,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1516,7 +1517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="3" borderId="0" xfId="23" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="3" borderId="0" xfId="23" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="33" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1861,7 +1862,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="$A8:$XFD11 $A2:$XFD2 $A1:$XFD1"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75"/>
@@ -3108,8 +3109,8 @@
   <sheetPr/>
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5:P5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A4:$XFD4 $A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75"/>
@@ -3560,14 +3561,19 @@
   <sheetPr/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88888888888889" style="2"/>
+    <col min="1" max="1" width="19.6666666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.66666666666667" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.22222222222222" style="2" customWidth="1"/>
+    <col min="4" max="5" width="6.22222222222222" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.66666666666667" style="2" customWidth="1"/>
+    <col min="7" max="9" width="6.22222222222222" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88888888888889" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3629,7 +3635,7 @@
         <v>72.05</v>
       </c>
       <c r="F3" s="10">
-        <v>62</v>
+        <v>66.1</v>
       </c>
       <c r="G3" s="10">
         <v>4.3</v>
@@ -3638,7 +3644,7 @@
         <v>51.46</v>
       </c>
       <c r="I3" s="13">
-        <v>68.31</v>
+        <v>71.31</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3717,4 +3723,20 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>